<commit_message>
Add evidence for task A7-A16, B1-B2
</commit_message>
<xml_diff>
--- a/trulacgc-tcnetwork/evidence.xlsx
+++ b/trulacgc-tcnetwork/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27860" windowHeight="13100" activeTab="1"/>
+    <workbookView windowWidth="27880" windowHeight="13100" tabRatio="725" firstSheet="11" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="78">
   <si>
     <t>TeamName</t>
   </si>
@@ -154,10 +154,97 @@
     <t>3E59A2D190439E8C7757B49CFB89A6EEF1D9E720D9C56460233F69288D0E181F</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
+    <t>ibc/D7784AD6C5F9AA0A58CFD8953DC9172B73518B7F30FF5783B33F560E2D7EADE8</t>
+  </si>
+  <si>
+    <t>nft07b</t>
+  </si>
+  <si>
+    <t>ibc/D54814DB59C52BCBFE7DD6A61FF49D562339C04D74728A3A5C6E6560682A2C64</t>
+  </si>
+  <si>
+    <t>nft08</t>
+  </si>
+  <si>
+    <t>ibc/16B314EF2B7F4F351EFD98B9BEB64125869A3C18545A0A0B5D93C48F22426A50</t>
+  </si>
+  <si>
+    <t>nft09</t>
+  </si>
+  <si>
+    <t>ibc/E990126C206F23BA73731C3B0C4FE4CB4EA20A623A2D5824E72A25E0A24D7361</t>
+  </si>
+  <si>
+    <t>nft10</t>
+  </si>
+  <si>
+    <t>ibc/3512E16D948E548373D02925C497741A49850F1306F9CDE55C2FF79E415A7700</t>
+  </si>
+  <si>
+    <t>nft11b</t>
+  </si>
+  <si>
+    <t>ibc/A825BCC8A1C68B440DF82442E4EAD9A7EF652568FBA3594F0747248AE320E0E9</t>
+  </si>
+  <si>
+    <t>nft12</t>
+  </si>
+  <si>
+    <t>BFD6A31A1CA7AD72CC530FFC0AAE64B16BA10C43580C2F69A565F2EAC9FAAC28</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>D90528ADDF756491304BEB759E2CB437601F47A0E75F0EBD75ACA3C142A02F6B</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>84BCD223298C584111921CD57F51DCC711CD1ACCF7E5E86F60243A5AD80D93AD</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>16769ACE38F39F5A96B5F55A30460A2AF1C6552C6E405FA470C33C4ED97C4FEA</t>
+  </si>
+  <si>
+    <t>EEB4C67AAECCAB18E58084E6862C4447E3652F178EA98E97193503821A65EE23</t>
+  </si>
+  <si>
+    <t>0E31570FC8CF1A64372B5AC381879FAA92496468D372F52569820B203606CBEF</t>
+  </si>
+  <si>
+    <t>0E07A8865EF829CC28BD6F019919A378EB9EB122ADA3A240CA9CD8E1BB56BF47</t>
+  </si>
+  <si>
+    <t>C8E5B9D45F0D5134CE471220B4012BEB3E051CF193395BED1C385ECE9F8F9532</t>
+  </si>
+  <si>
+    <t>E989EB6471431D01D556ACFDB52A40666D7646BE5F7DB028AB8A0F857CB1FF2F</t>
+  </si>
+  <si>
+    <t>428B2DD6CF732CC208DBDF2C76C76C13F8681792C728026C3A0F9579A22CCDDD</t>
+  </si>
+  <si>
+    <t>716FF727B5BB5D947B868D94BD374C36BDFEE29695FFB90C23B0DE8A1FCA6842</t>
+  </si>
+  <si>
+    <t>373D6CB1032E37CB41DAE556205FECB0DFBD80C1132D056B784346C348883D90</t>
+  </si>
+  <si>
+    <t>03D869FDA865BA50E1274DA6118C9C168CCDC044C87A35F31CF528F8F74ADF77</t>
+  </si>
+  <si>
+    <t>0DCA8F59903E7F132C74C6495C278F4C2422B43F8B3033A77E4B84FADDF02150</t>
+  </si>
+  <si>
+    <t>79A5ED34D4BF65B732015E509D817B8A30E16BEB0F876F1BE55C0DBBEC602460</t>
+  </si>
+  <si>
+    <t>0DEE0FBA3E6C9495C514B7500A6EA230CFF117899DD259E5AD5B11609B595C4C</t>
   </si>
   <si>
     <t>tx hash on that chain</t>
@@ -167,6 +254,18 @@
   </si>
   <si>
     <t>tx hash on that chain	chain id</t>
+  </si>
+  <si>
+    <t>27DCA2C253F09EEB7011027A5798E75E6E3595F93C3CCE62C0A78371955E3B40</t>
+  </si>
+  <si>
+    <t>0AB88466ECEE09330410EC28E3B06BD12A5307846420CB9C1DD3B351AD04F39F</t>
+  </si>
+  <si>
+    <t>891D78D08E1E9B1913580A240261F853CBBB2DA369F4FEFBE8F15946D890F535</t>
+  </si>
+  <si>
+    <t>748319F1D488DFB1CFC736F834D378C8B4E4E47912166B6733C587AF762908E7</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
@@ -185,7 +284,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +299,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -208,17 +313,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -231,7 +353,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,14 +375,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -270,22 +399,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,31 +420,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,43 +470,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,133 +590,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,6 +683,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -594,15 +708,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,6 +759,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -662,164 +776,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -828,6 +933,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1194,7 +1300,7 @@
     <col min="2" max="2" width="37.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="41.53125" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.0546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="42.0546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="40.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.75" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.1328125" style="1" customWidth="1"/>
@@ -1227,25 +1333,25 @@
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1" spans="1:8">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1266,7 +1372,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1285,10 +1391,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1305,7 +1411,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1324,10 +1430,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1344,7 +1450,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1363,10 +1469,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1383,7 +1489,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1402,10 +1508,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1419,13 +1525,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.0078125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.4296875" style="1" customWidth="1"/>
@@ -1441,20 +1547,34 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" customHeight="1" spans="1:1">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1468,13 +1588,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.0078125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.4296875" style="1" customWidth="1"/>
@@ -1490,20 +1610,34 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
+        <v>57</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" customHeight="1" spans="1:1">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>59</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1517,13 +1651,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.0078125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.4296875" style="1" customWidth="1"/>
@@ -1539,20 +1673,34 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" customHeight="1" spans="1:1">
+        <v>62</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>63</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1566,13 +1714,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.0078125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.4296875" style="1" customWidth="1"/>
@@ -1588,20 +1736,34 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
+        <v>65</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" customHeight="1" spans="1:1">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>67</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1637,20 +1799,20 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1686,20 +1848,20 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1715,7 +1877,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -1774,20 +1936,20 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1823,20 +1985,20 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1853,7 +2015,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
@@ -1866,14 +2028,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" ht="16.4" customHeight="1" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>44</v>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1889,8 +2051,8 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
@@ -1905,12 +2067,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1942,12 +2104,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1979,12 +2141,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2284,7 +2446,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2323,7 +2485,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2342,10 +2504,10 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add evidence for task A17-A20
</commit_message>
<xml_diff>
--- a/trulacgc-tcnetwork/evidence.xlsx
+++ b/trulacgc-tcnetwork/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27880" windowHeight="13100" tabRatio="725" firstSheet="11" activeTab="22"/>
+    <workbookView windowWidth="27900" windowHeight="13100" tabRatio="725" firstSheet="11" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="95">
   <si>
     <t>TeamName</t>
   </si>
@@ -247,13 +247,64 @@
     <t>0DEE0FBA3E6C9495C514B7500A6EA230CFF117899DD259E5AD5B11609B595C4C</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
+    <t>3004ACE1CF48346312087170D086FFB297892805864DDD57DD5D5929FD5D9DA0</t>
+  </si>
+  <si>
+    <t>916C6FEB38D1A3B8EC97B810C6D14889B60FDF0218FFC997B6F2EEAC06F1E2C1</t>
+  </si>
+  <si>
+    <t>99440FF8CEDB7F66642D7FDF91ACEDDA36EE06FF18384DA7B8421251A7F852A7</t>
+  </si>
+  <si>
+    <t>484637FF89A2827C2C197DEE750BE3F43E1521AB606B6E26CCF4CA8352D36C90</t>
+  </si>
+  <si>
+    <t>149EAF9A68CD53E0F96916488F7228803968BE76DB8CC9C80854DB71439ACAE2</t>
+  </si>
+  <si>
+    <t>DD62C6DEA63AE2CF86232B2E28A62FFC286DCFAA0F673C777C6BFE2FF086BEBB</t>
+  </si>
+  <si>
+    <t>A6BA638C9C82C4A2C65298F52F8ABBF623532C5DBA30F48ED6C67E79F541606C</t>
+  </si>
+  <si>
+    <t>53E3B4FA8B9D7F7B9B63F0CB2B01C830C4E0858319D806EBF6A8B8C2F9C65193</t>
+  </si>
+  <si>
+    <t>8AED18A418F896217479779942234FBADC3CB86D90A1BE3AD6F44F1349EA7387</t>
+  </si>
+  <si>
+    <t>0AC0687A62B90776DCB3924EE0C618F6EFD9F8DAE903F5CA077C3F9EF98E71AA</t>
+  </si>
+  <si>
+    <t>E38AF34A0ECAB2AEEB662AC34022947AD6EA4790B94E74C88FF1B82AC32C274C</t>
+  </si>
+  <si>
+    <t>B155BF4D9172887B10FFB98E5E4C55B57551EDB8EC647A1A180FED36686F2597</t>
+  </si>
+  <si>
+    <t>32140A5CC1AA0B3490374188439940BFA6D5AFC18BD9DD44FC9B3AEF31596DC7</t>
+  </si>
+  <si>
+    <t>886C56CED2C6E4AD2A2416B1B7697113F51A82F9A2659600641642684F417C2F</t>
+  </si>
+  <si>
+    <t>1D20D512AE4E52A78BB3A3DB9618F59EF50E29008DB0DAC7E7B68011E2E917A5</t>
+  </si>
+  <si>
+    <t>52B7A5F3E9237F878B4B3C1D0C4C2BC56DCE4D4EBA7DED7FA9C096A419219462</t>
+  </si>
+  <si>
+    <t>AB7AEAB7D0D87891175E180DAB12924AC7102FA00349F8821FA34E4F9B9F2ABA</t>
+  </si>
+  <si>
+    <t>D3907C27497BCE92B8176CD0ACB4132DEAECD528EA66268464C7E2CBF75AA905</t>
+  </si>
+  <si>
+    <t>F70DF5F783A0EB663B4E49959E3CCC5F2BD8EC6A7C4FFA5BAC8121927D2442AD</t>
+  </si>
+  <si>
+    <t>22B326510B09ADCA2B59EE1E723AAE81B55C71AD107A49D5A4ABB9C1CBB3E4F0</t>
   </si>
   <si>
     <t>27DCA2C253F09EEB7011027A5798E75E6E3595F93C3CCE62C0A78371955E3B40</t>
@@ -279,10 +330,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -313,16 +364,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -337,18 +380,17 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -360,45 +402,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,8 +424,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,7 +486,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,37 +521,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,145 +695,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,6 +726,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -708,21 +774,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -779,142 +830,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1777,13 +1828,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.0078125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.4296875" style="1" customWidth="1"/>
@@ -1801,18 +1852,32 @@
       <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1" spans="1:2">
+      <c r="A3" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" customHeight="1" spans="1:1">
+      <c r="B3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>71</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1826,13 +1891,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.0078125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.4296875" style="1" customWidth="1"/>
@@ -1848,20 +1913,34 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
+        <v>73</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" customHeight="1" spans="1:1">
+        <v>74</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1914,13 +1993,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.0078125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.4296875" style="1" customWidth="1"/>
@@ -1936,20 +2015,50 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
+        <v>77</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" customHeight="1" spans="1:1">
+        <v>78</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1963,13 +2072,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.0078125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.4296875" style="1" customWidth="1"/>
@@ -1985,20 +2094,50 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" customHeight="1" spans="1:1">
+        <v>83</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" customHeight="1" spans="1:1">
+        <v>84</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>85</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2030,12 +2169,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +2190,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -2067,12 +2206,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2104,12 +2243,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2141,12 +2280,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add evidence for task B5,B6,B7
</commit_message>
<xml_diff>
--- a/trulacgc-tcnetwork/evidence.xlsx
+++ b/trulacgc-tcnetwork/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27900" windowHeight="13100" tabRatio="725" firstSheet="11" activeTab="20"/>
+    <workbookView windowWidth="27880" windowHeight="13100" tabRatio="725" firstSheet="12" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -32,13 +32,14 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="99">
   <si>
     <t>TeamName</t>
   </si>
@@ -319,10 +320,22 @@
     <t>748319F1D488DFB1CFC736F834D378C8B4E4E47912166B6733C587AF762908E7</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
+    <t>EC916C28FEDC26EF04B221269A19ED7970A1427961D80814E82AC3E4ED18C66C</t>
+  </si>
+  <si>
+    <t>2736CADB22B48E9AE1F8AB7F61EDD18AB5E0CA8B8D2E872686A0279CD97AB358</t>
+  </si>
+  <si>
+    <t>BDE284C1812E0EF2C72E39CAF023A49E6AF6504B46119140CA2DA1B4424641B8</t>
+  </si>
+  <si>
+    <t>FE31A7197D5ABA789DDA7F5A10598532ACC2E83280999060413863867DFF4D2F</t>
+  </si>
+  <si>
+    <t>B9B9F4F81F3089C7AC6C66980E8E71504B9DB870C85D403E2A72411AE12DFF5F</t>
+  </si>
+  <si>
+    <t>7F680819B3F9324AE64FDB4E9F0E16B166E54E830E113F0CD02D620F38680644</t>
   </si>
 </sst>
 </file>
@@ -331,9 +344,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -364,21 +377,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -388,29 +386,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -426,6 +402,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -433,14 +424,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,6 +440,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,10 +475,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -486,15 +492,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -521,187 +534,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -730,35 +743,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -779,6 +768,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -789,6 +793,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,15 +823,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -827,145 +831,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2074,7 +2087,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -2228,7 +2241,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
@@ -2265,7 +2278,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
@@ -2280,12 +2293,49 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="12.4296875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="17.25" customHeight="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="17.25" customHeight="1" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" customHeight="1" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>